<commit_message>
Category Feed - Envelopes Categories
</commit_message>
<xml_diff>
--- a/src/CATEGORIES.xlsx
+++ b/src/CATEGORIES.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevStudio\Downloads\Data\PIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevStudio\Projects\Bigname\PIM\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FFE17C-A407-45C3-A69F-732140F4B510}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F073CA-DA40-4A92-B4BD-96FB87880C43}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14589" xr2:uid="{C7C2B3F2-E933-47B0-B644-4541E6AF93CE}"/>
   </bookViews>
@@ -660,9 +660,6 @@
     <t>Jiffylite Bubble®</t>
   </si>
   <si>
-    <t>EXTENRAL_ID</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -670,6 +667,9 @@
   </si>
   <si>
     <t>PARENT_ID</t>
+  </si>
+  <si>
+    <t>CATEGORY_ID</t>
   </si>
 </sst>
 </file>
@@ -1038,16 +1038,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" t="s">
         <v>209</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" t="s">
         <v>210</v>
-      </c>
-      <c r="C1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>